<commit_message>
Madhu- Intermediate working files
</commit_message>
<xml_diff>
--- a/dataforfinalproject/RawDataFiles/Codebooks/COMAPRE.xlsx
+++ b/dataforfinalproject/RawDataFiles/Codebooks/COMAPRE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SMU DS Bootcamp\Projects\Project3-ML_ResPoweConsumption\Project3final\dataforfinalproject\RawDataFiles\Codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4612DF-BEA1-42AE-A398-D33EB0BC52DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B155990-FDC6-45CC-B70A-9AD79BD9D4B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15200" windowHeight="6930" activeTab="2" xr2:uid="{4B938452-2864-46B4-89EF-E66CCA501EFB}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2540" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2598" uniqueCount="552">
   <si>
     <t>REGIONC</t>
   </si>
@@ -1589,9 +1589,6 @@
   </si>
   <si>
     <t>YearMade is converted to a range as per 2015 standards</t>
-  </si>
-  <si>
-    <t>Impute</t>
   </si>
   <si>
     <t>Drop 1997</t>
@@ -1773,12 +1770,147 @@
 NHAFBATH,
 OTHROOMS)</t>
   </si>
+  <si>
+    <t xml:space="preserve">BTUELAPL 
+BTUELRFG 
+BTUELFZZ 
+BTUELCOL
+BTUELDWH 
+BTUELCDR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOLELAPL 
+DOLELFZZ 
+DOLELCOL
+DOLELCDR 
+DOLELDWH </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOLELAPL 
+DOLELFZZ 
+DOLELCOL 
+DOLELCDR 
+DOLELDWH </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum(NUMPC
+LAPTOPPC
+PCPRINT
+FXCOPIER
+FAX
+COPIER)
+</t>
+  </si>
+  <si>
+    <t>HD65</t>
+  </si>
+  <si>
+    <t>Householder_Race</t>
+  </si>
+  <si>
+    <t>BTUFOOTH</t>
+  </si>
+  <si>
+    <t>Portable electric heater
+Wood-burning stove (cordwood or pellets)
+Natural gas fireplace
+Wood-burning fireplace
+Some other equipment
+Not applicable</t>
+  </si>
+  <si>
+    <t>Natural gas from underground pipes
+Propane (bottled gas)
+Fuel oil/kerosene
+Electricity
+Wood (cordwood or pellets)
+Some other fuel
+Not applicable</t>
+  </si>
+  <si>
+    <t>dropped</t>
+  </si>
+  <si>
+    <t>DOLELRFG1</t>
+  </si>
+  <si>
+    <t>DOLELRFG2</t>
+  </si>
+  <si>
+    <t>DOLELFRZ</t>
+  </si>
+  <si>
+    <t>DOLELCOK</t>
+  </si>
+  <si>
+    <t>DOLELMICRO</t>
+  </si>
+  <si>
+    <t>DOLELCW</t>
+  </si>
+  <si>
+    <t>DOLELCDR</t>
+  </si>
+  <si>
+    <t>DOLELDWH</t>
+  </si>
+  <si>
+    <t>DOLELLGT</t>
+  </si>
+  <si>
+    <t>DOLELTVREL</t>
+  </si>
+  <si>
+    <t>DOLELTV1</t>
+  </si>
+  <si>
+    <t>DOLELTV2</t>
+  </si>
+  <si>
+    <t>DOLELAHUHEAT</t>
+  </si>
+  <si>
+    <t>DOLELAHUCOL</t>
+  </si>
+  <si>
+    <t>DOLELCFAN</t>
+  </si>
+  <si>
+    <t>DOLELDHUM</t>
+  </si>
+  <si>
+    <t>DOLELHUM</t>
+  </si>
+  <si>
+    <t>DOLELPLPMP</t>
+  </si>
+  <si>
+    <t>DOLELHTBPMP</t>
+  </si>
+  <si>
+    <t>DOLELHTBHEAT</t>
+  </si>
+  <si>
+    <t>DOLELNEC</t>
+  </si>
+  <si>
+    <t>BTUFOWTH
+BTUKRWTH</t>
+  </si>
+  <si>
+    <t>BTUFOSPH
+BTUKRSPH</t>
+  </si>
+  <si>
+    <t>BTUFOAPL
+BTUKRAPL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1786,8 +1918,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1824,6 +1983,28 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1843,10 +2024,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1868,6 +2051,22 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1883,32 +2082,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral 2" xfId="2" xr:uid="{AF2F03F3-12C6-4E4E-B43D-0A3AE1DAB57D}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -2255,8 +2453,8 @@
   <dimension ref="A1:I355"/>
   <sheetViews>
     <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="1" x14ac:dyDescent="0.35"/>
@@ -3267,63 +3465,63 @@
       <c r="A77" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C77" s="16" t="s">
+      <c r="C77" s="24" t="s">
         <v>423</v>
       </c>
-      <c r="D77" s="16"/>
-      <c r="E77" s="16"/>
-      <c r="F77" s="16"/>
-      <c r="G77" s="16"/>
+      <c r="D77" s="24"/>
+      <c r="E77" s="24"/>
+      <c r="F77" s="24"/>
+      <c r="G77" s="24"/>
     </row>
     <row r="78" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C78" s="16"/>
-      <c r="D78" s="16"/>
-      <c r="E78" s="16"/>
-      <c r="F78" s="16"/>
-      <c r="G78" s="16"/>
+      <c r="C78" s="24"/>
+      <c r="D78" s="24"/>
+      <c r="E78" s="24"/>
+      <c r="F78" s="24"/>
+      <c r="G78" s="24"/>
     </row>
     <row r="79" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C79" s="16"/>
-      <c r="D79" s="16"/>
-      <c r="E79" s="16"/>
-      <c r="F79" s="16"/>
-      <c r="G79" s="16"/>
+      <c r="C79" s="24"/>
+      <c r="D79" s="24"/>
+      <c r="E79" s="24"/>
+      <c r="F79" s="24"/>
+      <c r="G79" s="24"/>
     </row>
     <row r="80" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C80" s="16"/>
-      <c r="D80" s="16"/>
-      <c r="E80" s="16"/>
-      <c r="F80" s="16"/>
-      <c r="G80" s="16"/>
+      <c r="C80" s="24"/>
+      <c r="D80" s="24"/>
+      <c r="E80" s="24"/>
+      <c r="F80" s="24"/>
+      <c r="G80" s="24"/>
     </row>
     <row r="81" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C81" s="16"/>
-      <c r="D81" s="16"/>
-      <c r="E81" s="16"/>
-      <c r="F81" s="16"/>
-      <c r="G81" s="16"/>
+      <c r="C81" s="24"/>
+      <c r="D81" s="24"/>
+      <c r="E81" s="24"/>
+      <c r="F81" s="24"/>
+      <c r="G81" s="24"/>
     </row>
     <row r="82" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C82" s="16"/>
-      <c r="D82" s="16"/>
-      <c r="E82" s="16"/>
-      <c r="F82" s="16"/>
-      <c r="G82" s="16"/>
+      <c r="C82" s="24"/>
+      <c r="D82" s="24"/>
+      <c r="E82" s="24"/>
+      <c r="F82" s="24"/>
+      <c r="G82" s="24"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
@@ -3416,12 +3614,12 @@
       <c r="B92" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="C92" s="13" t="s">
+      <c r="C92" s="21" t="s">
         <v>425</v>
       </c>
-      <c r="D92" s="13"/>
-      <c r="E92" s="13"/>
-      <c r="F92" s="13"/>
+      <c r="D92" s="21"/>
+      <c r="E92" s="21"/>
+      <c r="F92" s="21"/>
       <c r="G92" s="5" t="s">
         <v>89</v>
       </c>
@@ -3430,12 +3628,12 @@
       <c r="A93" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C93" s="13" t="s">
+      <c r="C93" s="21" t="s">
         <v>425</v>
       </c>
-      <c r="D93" s="13"/>
-      <c r="E93" s="13"/>
-      <c r="F93" s="13"/>
+      <c r="D93" s="21"/>
+      <c r="E93" s="21"/>
+      <c r="F93" s="21"/>
       <c r="G93" s="5" t="s">
         <v>90</v>
       </c>
@@ -4129,13 +4327,13 @@
       <c r="A156" t="s">
         <v>153</v>
       </c>
-      <c r="C156" s="17" t="s">
+      <c r="C156" s="25" t="s">
         <v>442</v>
       </c>
-      <c r="D156" s="17"/>
-      <c r="E156" s="17"/>
-      <c r="F156" s="17"/>
-      <c r="G156" s="17"/>
+      <c r="D156" s="25"/>
+      <c r="E156" s="25"/>
+      <c r="F156" s="25"/>
+      <c r="G156" s="25"/>
     </row>
     <row r="157" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
@@ -5331,7 +5529,7 @@
       </c>
     </row>
     <row r="308" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B308" s="13" t="s">
+      <c r="B308" s="21" t="s">
         <v>450</v>
       </c>
       <c r="C308" s="5" t="s">
@@ -5343,15 +5541,15 @@
       <c r="E308" s="5" t="s">
         <v>451</v>
       </c>
-      <c r="F308" s="13" t="s">
+      <c r="F308" s="21" t="s">
         <v>450</v>
       </c>
-      <c r="G308" s="14" t="s">
+      <c r="G308" s="22" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="309" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B309" s="13"/>
+      <c r="B309" s="21"/>
       <c r="C309" s="5" t="s">
         <v>452</v>
       </c>
@@ -5361,8 +5559,8 @@
       <c r="E309" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="F309" s="13"/>
-      <c r="G309" s="13"/>
+      <c r="F309" s="21"/>
+      <c r="G309" s="21"/>
     </row>
     <row r="310" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B310" s="5" t="s">
@@ -5798,52 +5996,52 @@
       <c r="A342" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="H342" s="15" t="s">
+      <c r="H342" s="23" t="s">
         <v>487</v>
       </c>
-      <c r="I342" s="15"/>
+      <c r="I342" s="23"/>
     </row>
     <row r="343" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A343" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="H343" s="15"/>
-      <c r="I343" s="15"/>
+      <c r="H343" s="23"/>
+      <c r="I343" s="23"/>
     </row>
     <row r="344" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A344" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="H344" s="15"/>
-      <c r="I344" s="15"/>
+      <c r="H344" s="23"/>
+      <c r="I344" s="23"/>
     </row>
     <row r="345" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A345" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="H345" s="15"/>
-      <c r="I345" s="15"/>
+      <c r="H345" s="23"/>
+      <c r="I345" s="23"/>
     </row>
     <row r="346" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A346" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="H346" s="15"/>
-      <c r="I346" s="15"/>
+      <c r="H346" s="23"/>
+      <c r="I346" s="23"/>
     </row>
     <row r="347" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A347" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="H347" s="15"/>
-      <c r="I347" s="15"/>
+      <c r="H347" s="23"/>
+      <c r="I347" s="23"/>
     </row>
     <row r="348" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A348" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="H348" s="15"/>
-      <c r="I348" s="15"/>
+      <c r="H348" s="23"/>
+      <c r="I348" s="23"/>
     </row>
     <row r="349" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A349" s="3" t="s">
@@ -7423,13 +7621,13 @@
       <c r="A107" t="s">
         <v>153</v>
       </c>
-      <c r="C107" s="17" t="s">
+      <c r="C107" s="25" t="s">
         <v>442</v>
       </c>
-      <c r="D107" s="17"/>
-      <c r="E107" s="17"/>
-      <c r="F107" s="17"/>
-      <c r="G107" s="17"/>
+      <c r="D107" s="25"/>
+      <c r="E107" s="25"/>
+      <c r="F107" s="25"/>
+      <c r="G107" s="25"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
@@ -7980,14 +8178,15 @@
   <dimension ref="A1:I187"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C111" sqref="C111"/>
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B148" sqref="B148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="15.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="19.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="81.7265625" bestFit="1" customWidth="1"/>
@@ -8116,16 +8315,16 @@
         <v>327</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>409</v>
+        <v>327</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>3</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -8187,7 +8386,7 @@
       <c r="F9" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="18" t="s">
         <v>6</v>
       </c>
     </row>
@@ -8204,10 +8403,10 @@
       <c r="E10" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>412</v>
-      </c>
-      <c r="G10" s="4" t="s">
+      <c r="F10" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="18" t="s">
         <v>7</v>
       </c>
     </row>
@@ -8310,6 +8509,7 @@
       <c r="C15" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="D15" s="19"/>
       <c r="E15" s="4" t="s">
         <v>12</v>
       </c>
@@ -8416,8 +8616,8 @@
       <c r="E20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>22</v>
+      <c r="F20" s="18" t="s">
+        <v>367</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>22</v>
@@ -8683,10 +8883,10 @@
       <c r="C32" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="18" t="s">
         <v>415</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="18" t="s">
         <v>415</v>
       </c>
       <c r="F32" s="4" t="s">
@@ -9037,7 +9237,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>87</v>
       </c>
@@ -9060,7 +9260,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>88</v>
       </c>
@@ -9083,53 +9283,65 @@
         <v>88</v>
       </c>
     </row>
-    <row r="51" spans="1:7" s="4" customFormat="1" ht="174" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" s="4" customFormat="1" ht="174" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B51" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="C51" s="27" t="s">
+      <c r="B51" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C51" s="17" t="s">
         <v>425</v>
       </c>
-      <c r="D51" s="19" t="s">
-        <v>515</v>
-      </c>
-      <c r="E51" s="19" t="s">
-        <v>515</v>
-      </c>
-      <c r="F51" s="19" t="s">
-        <v>513</v>
-      </c>
-      <c r="G51" s="4" t="s">
+      <c r="D51" s="27" t="s">
+        <v>514</v>
+      </c>
+      <c r="E51" s="27" t="s">
+        <v>514</v>
+      </c>
+      <c r="F51" s="27" t="s">
+        <v>512</v>
+      </c>
+      <c r="G51" s="18" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" s="4" customFormat="1" ht="116" x14ac:dyDescent="0.35">
+      <c r="H51" s="20" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" s="4" customFormat="1" ht="116" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C52" s="27" t="s">
+      <c r="B52" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C52" s="17" t="s">
         <v>425</v>
       </c>
-      <c r="D52" s="19" t="s">
-        <v>516</v>
-      </c>
-      <c r="E52" s="19" t="s">
-        <v>516</v>
-      </c>
-      <c r="F52" s="19" t="s">
-        <v>514</v>
-      </c>
-      <c r="G52" s="4" t="s">
+      <c r="D52" s="27" t="s">
+        <v>515</v>
+      </c>
+      <c r="E52" s="27" t="s">
+        <v>515</v>
+      </c>
+      <c r="F52" s="27" t="s">
+        <v>513</v>
+      </c>
+      <c r="G52" s="18" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="H52" s="26" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>91</v>
       </c>
+      <c r="B53" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="D53" s="4" t="s">
         <v>91</v>
       </c>
@@ -9143,10 +9355,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
         <v>92</v>
       </c>
+      <c r="B54" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="D54" s="4" t="s">
         <v>92</v>
       </c>
@@ -9160,7 +9375,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>94</v>
       </c>
@@ -9183,7 +9398,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>95</v>
       </c>
@@ -9206,7 +9421,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>96</v>
       </c>
@@ -9229,7 +9444,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>97</v>
       </c>
@@ -9252,7 +9467,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>98</v>
       </c>
@@ -9275,7 +9490,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>99</v>
       </c>
@@ -9298,7 +9513,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>100</v>
       </c>
@@ -9321,7 +9536,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>104</v>
       </c>
@@ -9344,7 +9559,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>105</v>
       </c>
@@ -9367,7 +9582,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>106</v>
       </c>
@@ -9394,19 +9609,22 @@
       <c r="A65" s="4" t="s">
         <v>114</v>
       </c>
+      <c r="B65" s="18" t="s">
+        <v>114</v>
+      </c>
       <c r="C65" s="4" t="s">
         <v>429</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="D65" s="18" t="s">
+        <v>429</v>
+      </c>
+      <c r="E65" s="18" t="s">
         <v>430</v>
       </c>
-      <c r="E65" s="4" t="s">
+      <c r="F65" s="18" t="s">
         <v>430</v>
       </c>
-      <c r="F65" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="G65" s="4" t="s">
+      <c r="G65" s="18" t="s">
         <v>114</v>
       </c>
     </row>
@@ -9414,11 +9632,11 @@
       <c r="A66" s="4" t="s">
         <v>118</v>
       </c>
+      <c r="B66" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="C66" s="4" t="s">
         <v>431</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>495</v>
       </c>
       <c r="E66" s="4" t="s">
         <v>118</v>
@@ -9434,6 +9652,9 @@
       <c r="A67" s="4" t="s">
         <v>126</v>
       </c>
+      <c r="B67" s="4" t="s">
+        <v>434</v>
+      </c>
       <c r="C67" s="4" t="s">
         <v>434</v>
       </c>
@@ -9454,6 +9675,9 @@
       <c r="A68" s="4" t="s">
         <v>127</v>
       </c>
+      <c r="B68" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="C68" s="4" t="s">
         <v>435</v>
       </c>
@@ -9474,6 +9698,9 @@
       <c r="A69" s="4" t="s">
         <v>128</v>
       </c>
+      <c r="B69" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="C69" s="4" t="s">
         <v>436</v>
       </c>
@@ -9563,19 +9790,22 @@
       <c r="A73" s="4" t="s">
         <v>135</v>
       </c>
+      <c r="B73" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C73" s="4" t="s">
         <v>437</v>
       </c>
-      <c r="D73" s="4" t="s">
+      <c r="D73" s="18" t="s">
         <v>438</v>
       </c>
-      <c r="E73" s="4" t="s">
+      <c r="E73" s="18" t="s">
         <v>438</v>
       </c>
-      <c r="F73" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="G73" s="4" t="s">
+      <c r="F73" s="18" t="s">
+        <v>523</v>
+      </c>
+      <c r="G73" s="18" t="s">
         <v>135</v>
       </c>
     </row>
@@ -9698,6 +9928,9 @@
       <c r="A79" s="4" t="s">
         <v>147</v>
       </c>
+      <c r="B79" s="4" t="s">
+        <v>147</v>
+      </c>
       <c r="D79" s="4" t="s">
         <v>147</v>
       </c>
@@ -9715,6 +9948,9 @@
       <c r="A80" s="4" t="s">
         <v>148</v>
       </c>
+      <c r="B80" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="D80" s="4" t="s">
         <v>148</v>
       </c>
@@ -9729,20 +9965,25 @@
       </c>
     </row>
     <row r="81" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="4" t="s">
+      <c r="A81" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="D81" s="4" t="s">
+      <c r="B81" s="28"/>
+      <c r="C81" s="28"/>
+      <c r="D81" s="28" t="s">
         <v>441</v>
       </c>
-      <c r="E81" s="4" t="s">
+      <c r="E81" s="28" t="s">
         <v>441</v>
       </c>
-      <c r="F81" s="4" t="s">
+      <c r="F81" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="G81" s="4" t="s">
+      <c r="G81" s="28" t="s">
         <v>149</v>
+      </c>
+      <c r="H81" s="28" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="82" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -9792,16 +10033,16 @@
       <c r="C84" t="s">
         <v>250</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D84" s="18" t="s">
         <v>250</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E84" s="18" t="s">
         <v>443</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F84" s="18" t="s">
         <v>250</v>
       </c>
-      <c r="G84" t="s">
+      <c r="G84" s="18" t="s">
         <v>250</v>
       </c>
     </row>
@@ -9812,16 +10053,16 @@
       <c r="C85" t="s">
         <v>444</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D85" s="18" t="s">
         <v>444</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E85" s="18" t="s">
+        <v>522</v>
+      </c>
+      <c r="F85" s="18" t="s">
         <v>444</v>
       </c>
-      <c r="F85" t="s">
-        <v>444</v>
-      </c>
-      <c r="G85" t="s">
+      <c r="G85" s="18" t="s">
         <v>444</v>
       </c>
     </row>
@@ -9836,7 +10077,7 @@
         <v>444</v>
       </c>
       <c r="E86" t="s">
-        <v>444</v>
+        <v>522</v>
       </c>
       <c r="F86" t="s">
         <v>444</v>
@@ -10010,22 +10251,22 @@
       </c>
     </row>
     <row r="94" spans="1:8" s="4" customFormat="1" ht="319" x14ac:dyDescent="0.35">
-      <c r="B94" s="4" t="s">
+      <c r="B94" s="18" t="s">
         <v>448</v>
       </c>
-      <c r="C94" s="19" t="s">
+      <c r="C94" s="27" t="s">
         <v>471</v>
       </c>
-      <c r="D94" s="19" t="s">
-        <v>471</v>
-      </c>
-      <c r="E94" s="19" t="s">
-        <v>471</v>
-      </c>
-      <c r="F94" s="20" t="s">
+      <c r="D94" s="27" t="s">
+        <v>518</v>
+      </c>
+      <c r="E94" s="27" t="s">
+        <v>518</v>
+      </c>
+      <c r="F94" s="29" t="s">
         <v>448</v>
       </c>
-      <c r="G94" s="19" t="s">
+      <c r="G94" s="27" t="s">
         <v>470</v>
       </c>
     </row>
@@ -10090,22 +10331,22 @@
       </c>
     </row>
     <row r="98" spans="1:9" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B98" s="4" t="s">
+      <c r="B98" s="18" t="s">
+        <v>455</v>
+      </c>
+      <c r="C98" s="18" t="s">
         <v>454</v>
       </c>
-      <c r="C98" s="4" t="s">
+      <c r="D98" s="18" t="s">
         <v>454</v>
       </c>
-      <c r="D98" s="4" t="s">
+      <c r="E98" s="18" t="s">
         <v>454</v>
       </c>
-      <c r="E98" s="4" t="s">
-        <v>454</v>
-      </c>
-      <c r="F98" s="4" t="s">
+      <c r="F98" s="18" t="s">
         <v>455</v>
       </c>
-      <c r="G98" s="19" t="s">
+      <c r="G98" s="27" t="s">
         <v>456</v>
       </c>
     </row>
@@ -10170,38 +10411,34 @@
       </c>
     </row>
     <row r="102" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B102" s="18" t="s">
+      <c r="B102" s="30" t="s">
         <v>450</v>
       </c>
-      <c r="C102" s="4" t="s">
+      <c r="C102" s="18" t="s">
         <v>451</v>
       </c>
-      <c r="D102" s="4" t="s">
+      <c r="D102" s="30" t="s">
         <v>451</v>
       </c>
-      <c r="E102" s="4" t="s">
+      <c r="E102" s="30" t="s">
         <v>451</v>
       </c>
-      <c r="F102" s="18" t="s">
+      <c r="F102" s="30" t="s">
         <v>450</v>
       </c>
-      <c r="G102" s="21" t="s">
+      <c r="G102" s="31" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="103" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B103" s="18"/>
-      <c r="C103" s="4" t="s">
+      <c r="B103" s="30"/>
+      <c r="C103" s="18" t="s">
         <v>452</v>
       </c>
-      <c r="D103" s="4" t="s">
-        <v>452</v>
-      </c>
-      <c r="E103" s="4" t="s">
-        <v>452</v>
-      </c>
-      <c r="F103" s="18"/>
-      <c r="G103" s="18"/>
+      <c r="D103" s="30"/>
+      <c r="E103" s="30"/>
+      <c r="F103" s="30"/>
+      <c r="G103" s="30"/>
     </row>
     <row r="104" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B104" s="4" t="s">
@@ -10223,15 +10460,15 @@
         <v>399</v>
       </c>
     </row>
-    <row r="105" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B105" s="4" t="s">
         <v>400</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="D105" s="4" t="s">
-        <v>400</v>
+      <c r="D105" s="13" t="s">
+        <v>550</v>
       </c>
       <c r="E105" s="4" t="s">
         <v>400</v>
@@ -10243,15 +10480,15 @@
         <v>400</v>
       </c>
     </row>
-    <row r="106" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B106" s="4" t="s">
         <v>401</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="D106" s="4" t="s">
-        <v>401</v>
+      <c r="D106" s="13" t="s">
+        <v>549</v>
       </c>
       <c r="E106" s="4" t="s">
         <v>401</v>
@@ -10263,28 +10500,28 @@
         <v>401</v>
       </c>
     </row>
-    <row r="107" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="22"/>
-      <c r="B107" s="22" t="s">
+    <row r="107" spans="1:9" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A107" s="14"/>
+      <c r="B107" s="32" t="s">
+        <v>524</v>
+      </c>
+      <c r="C107" s="32" t="s">
         <v>457</v>
       </c>
-      <c r="C107" s="22" t="s">
+      <c r="D107" s="33" t="s">
+        <v>551</v>
+      </c>
+      <c r="E107" s="32" t="s">
         <v>457</v>
       </c>
-      <c r="D107" s="22" t="s">
-        <v>457</v>
-      </c>
-      <c r="E107" s="22" t="s">
-        <v>457</v>
-      </c>
-      <c r="F107" s="22" t="s">
-        <v>458</v>
-      </c>
-      <c r="G107" s="22" t="s">
+      <c r="F107" s="32" t="s">
+        <v>524</v>
+      </c>
+      <c r="G107" s="32" t="s">
         <v>459</v>
       </c>
-      <c r="H107" s="22"/>
-      <c r="I107" s="22"/>
+      <c r="H107" s="14"/>
+      <c r="I107" s="14"/>
     </row>
     <row r="108" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A108" s="4" t="s">
@@ -10356,22 +10593,22 @@
       </c>
     </row>
     <row r="111" spans="1:9" s="4" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B111" s="4" t="s">
+      <c r="B111" s="18" t="s">
         <v>461</v>
       </c>
-      <c r="C111" s="19" t="s">
+      <c r="C111" s="27" t="s">
         <v>462</v>
       </c>
-      <c r="D111" s="4" t="s">
+      <c r="D111" s="18" t="s">
         <v>463</v>
       </c>
-      <c r="E111" s="4" t="s">
+      <c r="E111" s="18" t="s">
         <v>463</v>
       </c>
-      <c r="F111" s="4" t="s">
+      <c r="F111" s="18" t="s">
         <v>461</v>
       </c>
-      <c r="G111" s="19" t="s">
+      <c r="G111" s="27" t="s">
         <v>460</v>
       </c>
     </row>
@@ -10491,22 +10728,22 @@
       </c>
     </row>
     <row r="117" spans="1:9" s="4" customFormat="1" ht="304.5" x14ac:dyDescent="0.35">
-      <c r="B117" s="4" t="s">
+      <c r="B117" s="18" t="s">
         <v>477</v>
       </c>
-      <c r="C117" s="19" t="s">
+      <c r="C117" s="27" t="s">
         <v>478</v>
       </c>
-      <c r="D117" s="19" t="s">
-        <v>478</v>
-      </c>
-      <c r="E117" s="19" t="s">
-        <v>478</v>
-      </c>
-      <c r="F117" s="4" t="s">
-        <v>449</v>
-      </c>
-      <c r="G117" s="19" t="s">
+      <c r="D117" s="27" t="s">
+        <v>519</v>
+      </c>
+      <c r="E117" s="27" t="s">
+        <v>520</v>
+      </c>
+      <c r="F117" s="18" t="s">
+        <v>477</v>
+      </c>
+      <c r="G117" s="27" t="s">
         <v>479</v>
       </c>
     </row>
@@ -10580,22 +10817,22 @@
       </c>
     </row>
     <row r="121" spans="1:9" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B121" s="4" t="s">
+      <c r="B121" s="18" t="s">
         <v>465</v>
       </c>
-      <c r="C121" s="4" t="s">
+      <c r="C121" s="18" t="s">
         <v>466</v>
       </c>
-      <c r="D121" s="4" t="s">
+      <c r="D121" s="18" t="s">
         <v>466</v>
       </c>
-      <c r="E121" s="4" t="s">
+      <c r="E121" s="18" t="s">
         <v>466</v>
       </c>
-      <c r="F121" s="4" t="s">
+      <c r="F121" s="18" t="s">
         <v>465</v>
       </c>
-      <c r="G121" s="19" t="s">
+      <c r="G121" s="27" t="s">
         <v>464</v>
       </c>
     </row>
@@ -10620,67 +10857,67 @@
       </c>
     </row>
     <row r="123" spans="1:9" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="B123" s="4" t="s">
+      <c r="B123" s="18" t="s">
         <v>403</v>
       </c>
-      <c r="C123" s="19" t="s">
+      <c r="C123" s="27" t="s">
         <v>480</v>
       </c>
-      <c r="D123" s="19" t="s">
+      <c r="D123" s="27" t="s">
         <v>480</v>
       </c>
-      <c r="E123" s="4" t="s">
+      <c r="E123" s="18" t="s">
         <v>403</v>
       </c>
-      <c r="F123" s="4" t="s">
+      <c r="F123" s="18" t="s">
         <v>403</v>
       </c>
-      <c r="G123" s="4" t="s">
+      <c r="G123" s="18" t="s">
         <v>403</v>
       </c>
     </row>
     <row r="124" spans="1:9" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="B124" s="4" t="s">
+      <c r="B124" s="18" t="s">
         <v>404</v>
       </c>
-      <c r="C124" s="19" t="s">
+      <c r="C124" s="27" t="s">
         <v>481</v>
       </c>
-      <c r="D124" s="19" t="s">
+      <c r="D124" s="27" t="s">
         <v>481</v>
       </c>
-      <c r="E124" s="4" t="s">
+      <c r="E124" s="18" t="s">
         <v>404</v>
       </c>
-      <c r="F124" s="4" t="s">
+      <c r="F124" s="18" t="s">
         <v>404</v>
       </c>
-      <c r="G124" s="4" t="s">
+      <c r="G124" s="18" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="125" spans="1:9" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A125" s="22"/>
-      <c r="B125" s="22" t="s">
+      <c r="A125" s="14"/>
+      <c r="B125" s="32" t="s">
         <v>467</v>
       </c>
-      <c r="C125" s="23" t="s">
+      <c r="C125" s="33" t="s">
         <v>482</v>
       </c>
-      <c r="D125" s="23" t="s">
+      <c r="D125" s="33" t="s">
         <v>482</v>
       </c>
-      <c r="E125" s="22" t="s">
+      <c r="E125" s="32" t="s">
         <v>469</v>
       </c>
-      <c r="F125" s="22" t="s">
+      <c r="F125" s="32" t="s">
         <v>467</v>
       </c>
-      <c r="G125" s="24" t="s">
+      <c r="G125" s="34" t="s">
         <v>468</v>
       </c>
-      <c r="H125" s="22"/>
-      <c r="I125" s="22"/>
+      <c r="H125" s="14"/>
+      <c r="I125" s="14"/>
     </row>
     <row r="126" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="s">
@@ -10709,7 +10946,9 @@
       <c r="A127" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="B127" s="9"/>
+      <c r="B127" s="9" t="s">
+        <v>310</v>
+      </c>
       <c r="C127" s="9"/>
       <c r="D127" s="9"/>
       <c r="E127" s="9"/>
@@ -10724,7 +10963,9 @@
       <c r="A128" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="B128" s="9"/>
+      <c r="B128" s="9" t="s">
+        <v>311</v>
+      </c>
       <c r="C128" s="9"/>
       <c r="D128" s="9"/>
       <c r="E128" s="9"/>
@@ -10739,7 +10980,9 @@
       <c r="A129" s="9" t="s">
         <v>313</v>
       </c>
-      <c r="B129" s="9"/>
+      <c r="B129" s="9" t="s">
+        <v>313</v>
+      </c>
       <c r="C129" s="9"/>
       <c r="D129" s="9"/>
       <c r="E129" s="9"/>
@@ -10784,7 +11027,9 @@
       <c r="A132" s="9" t="s">
         <v>312</v>
       </c>
-      <c r="B132" s="9"/>
+      <c r="B132" s="9" t="s">
+        <v>312</v>
+      </c>
       <c r="C132" s="9"/>
       <c r="D132" s="9"/>
       <c r="E132" s="9"/>
@@ -10799,7 +11044,9 @@
       <c r="A133" s="9" t="s">
         <v>314</v>
       </c>
-      <c r="B133" s="9"/>
+      <c r="B133" s="9" t="s">
+        <v>314</v>
+      </c>
       <c r="C133" s="9"/>
       <c r="D133" s="9"/>
       <c r="E133" s="9"/>
@@ -11838,64 +12085,67 @@
       </c>
     </row>
     <row r="185" spans="2:7" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="B185" s="26" t="s">
-        <v>503</v>
-      </c>
-      <c r="D185" s="25" t="s">
-        <v>505</v>
-      </c>
-      <c r="E185" s="25" t="s">
+      <c r="B185" s="16" t="s">
         <v>502</v>
       </c>
-      <c r="F185" s="25" t="s">
+      <c r="D185" s="15" t="s">
+        <v>504</v>
+      </c>
+      <c r="E185" s="15" t="s">
+        <v>501</v>
+      </c>
+      <c r="F185" s="15" t="s">
+        <v>496</v>
+      </c>
+      <c r="G185" s="15" t="s">
         <v>497</v>
-      </c>
-      <c r="G185" s="25" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="186" spans="2:7" ht="145" x14ac:dyDescent="0.35">
       <c r="B186" t="s">
+        <v>498</v>
+      </c>
+      <c r="D186" s="15" t="s">
+        <v>521</v>
+      </c>
+      <c r="E186" s="15" t="s">
+        <v>503</v>
+      </c>
+      <c r="F186" s="15" t="s">
+        <v>500</v>
+      </c>
+      <c r="G186" s="15" t="s">
         <v>499</v>
-      </c>
-      <c r="D186" s="25" t="s">
-        <v>504</v>
-      </c>
-      <c r="E186" s="25" t="s">
-        <v>504</v>
-      </c>
-      <c r="F186" s="25" t="s">
-        <v>501</v>
-      </c>
-      <c r="G186" s="25" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="187" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B187" t="s">
+        <v>505</v>
+      </c>
+      <c r="D187" s="15" t="s">
         <v>506</v>
       </c>
-      <c r="D187" s="25" t="s">
+      <c r="E187" s="15" t="s">
         <v>507</v>
       </c>
-      <c r="E187" s="25" t="s">
+      <c r="F187" s="15" t="s">
+        <v>509</v>
+      </c>
+      <c r="G187" s="15" t="s">
         <v>508</v>
-      </c>
-      <c r="F187" s="25" t="s">
-        <v>510</v>
-      </c>
-      <c r="G187" s="25" t="s">
-        <v>509</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G139" xr:uid="{DC2F319F-5412-4A47-8C4C-6B3D4AB55F46}"/>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="B102:B103"/>
     <mergeCell ref="F102:F103"/>
     <mergeCell ref="G102:G103"/>
+    <mergeCell ref="D102:D103"/>
+    <mergeCell ref="E102:E103"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11903,8 +12153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B934CF8-43DC-4F81-B841-492EF34EF463}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11935,7 +12185,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -11943,7 +12193,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -11951,7 +12201,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -11959,12 +12209,12 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" s="9" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -12304,14 +12554,183 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8AE98A-036F-4E6F-82C6-B69D2EC4EAD3}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C1" sqref="C1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>528</v>
+      </c>
+      <c r="C1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D1" t="s">
+        <v>529</v>
+      </c>
+      <c r="E1" t="s">
+        <v>530</v>
+      </c>
+      <c r="F1" t="s">
+        <v>531</v>
+      </c>
+      <c r="G1" t="s">
+        <v>532</v>
+      </c>
+      <c r="H1" t="s">
+        <v>533</v>
+      </c>
+      <c r="I1" t="s">
+        <v>534</v>
+      </c>
+      <c r="J1" t="s">
+        <v>535</v>
+      </c>
+      <c r="K1" t="s">
+        <v>536</v>
+      </c>
+      <c r="L1" t="s">
+        <v>537</v>
+      </c>
+      <c r="M1" t="s">
+        <v>538</v>
+      </c>
+      <c r="N1" t="s">
+        <v>539</v>
+      </c>
+      <c r="O1" t="s">
+        <v>540</v>
+      </c>
+      <c r="P1" t="s">
+        <v>541</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>542</v>
+      </c>
+      <c r="R1" t="s">
+        <v>543</v>
+      </c>
+      <c r="S1" t="s">
+        <v>544</v>
+      </c>
+      <c r="T1" t="s">
+        <v>545</v>
+      </c>
+      <c r="U1" t="s">
+        <v>546</v>
+      </c>
+      <c r="V1" t="s">
+        <v>547</v>
+      </c>
+      <c r="W1" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>548</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>